<commit_message>
IAEMOD-10996: updated extract file
</commit_message>
<xml_diff>
--- a/_apidocs/sam-entity-extracts-api/v1/SAM Master Extract Mapping v7.0 Sensitive File V3 Layout.xlsx
+++ b/_apidocs/sam-entity-extracts-api/v1/SAM Master Extract Mapping v7.0 Sensitive File V3 Layout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\E04BMK-XDVCFP1\RedirAE$\jyothirmayichavali\Desktop\PI44\Iteration3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\E04BMK-XDVCFP1\RedirAE$\jyothirmayichavali\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E1AB3-F05D-45CD-A86F-0C1130BE77A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906CE479-7E23-4626-86A5-886E038A22E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3084" uniqueCount="926">
   <si>
     <t>SAM DATA ELEMENT LIST</t>
   </si>
@@ -2850,6 +2850,9 @@
   </si>
   <si>
     <t>Sensitive (CUI)</t>
+  </si>
+  <si>
+    <t>Blank Spaces, formerly occupied by the MPIN</t>
   </si>
 </sst>
 </file>
@@ -3612,7 +3615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3972,19 +3975,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4258,10 +4252,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B279" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K288" sqref="K288:O288"/>
+      <selection pane="bottomRight" activeCell="O288" sqref="O288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
@@ -4300,23 +4294,23 @@
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
-      <c r="O2" s="132"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="129"/>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1">
       <c r="A3" s="6" t="s">
@@ -4325,23 +4319,23 @@
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="136" t="s">
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="137"/>
-      <c r="M3" s="137"/>
-      <c r="N3" s="137"/>
-      <c r="O3" s="138"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="134"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="135"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="8" t="s">
@@ -17830,32 +17824,32 @@
       <c r="E288" s="124">
         <v>9</v>
       </c>
-      <c r="F288" s="125" t="s">
-        <v>27</v>
+      <c r="F288" s="26" t="s">
+        <v>925</v>
       </c>
       <c r="G288" s="19"/>
-      <c r="H288" s="126" t="s">
+      <c r="H288" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="I288" s="126"/>
-      <c r="J288" s="127" t="s">
+      <c r="I288" s="125"/>
+      <c r="J288" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="K288" s="123" t="s">
+      <c r="K288" s="19" t="s">
         <v>924</v>
       </c>
-      <c r="L288" s="127">
+      <c r="L288" s="19">
         <v>3</v>
       </c>
-      <c r="M288" s="128" t="str">
+      <c r="M288" s="126" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="N288" s="128" t="str">
+      <c r="N288" s="126" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="O288" s="129" t="str">
+      <c r="O288" s="34" t="str">
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
@@ -22356,10 +22350,10 @@
       <c r="B5" s="68" t="s">
         <v>587</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="138" t="s">
         <v>588</v>
       </c>
-      <c r="D5" s="142"/>
+      <c r="D5" s="139"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
         <v>589</v>
@@ -22528,10 +22522,10 @@
       <c r="B10" s="69" t="s">
         <v>594</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="140" t="s">
         <v>595</v>
       </c>
-      <c r="D10" s="144"/>
+      <c r="D10" s="141"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
         <v>596</v>
@@ -22702,10 +22696,10 @@
       <c r="B15" s="69" t="s">
         <v>600</v>
       </c>
-      <c r="C15" s="143" t="s">
+      <c r="C15" s="140" t="s">
         <v>601</v>
       </c>
-      <c r="D15" s="144"/>
+      <c r="D15" s="141"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -22878,10 +22872,10 @@
       <c r="B20" s="69" t="s">
         <v>607</v>
       </c>
-      <c r="C20" s="143" t="s">
+      <c r="C20" s="140" t="s">
         <v>608</v>
       </c>
-      <c r="D20" s="144"/>
+      <c r="D20" s="141"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
         <v>609</v>
@@ -23052,10 +23046,10 @@
       <c r="B25" s="69" t="s">
         <v>613</v>
       </c>
-      <c r="C25" s="143" t="s">
+      <c r="C25" s="140" t="s">
         <v>614</v>
       </c>
-      <c r="D25" s="144"/>
+      <c r="D25" s="141"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
         <v>615</v>
@@ -26914,13 +26908,13 @@
     <row r="148" spans="1:26" ht="12.75" customHeight="1">
       <c r="A148" s="5"/>
       <c r="B148" s="5"/>
-      <c r="C148" s="139" t="s">
+      <c r="C148" s="136" t="s">
         <v>812</v>
       </c>
-      <c r="D148" s="140"/>
-      <c r="E148" s="140"/>
-      <c r="F148" s="140"/>
-      <c r="G148" s="140"/>
+      <c r="D148" s="137"/>
+      <c r="E148" s="137"/>
+      <c r="F148" s="137"/>
+      <c r="G148" s="137"/>
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
       <c r="J148" s="5"/>
@@ -26944,13 +26938,13 @@
     <row r="149" spans="1:26" ht="75.75" customHeight="1">
       <c r="A149" s="5"/>
       <c r="B149" s="5"/>
-      <c r="C149" s="139" t="s">
+      <c r="C149" s="136" t="s">
         <v>813</v>
       </c>
-      <c r="D149" s="140"/>
-      <c r="E149" s="140"/>
-      <c r="F149" s="140"/>
-      <c r="G149" s="140"/>
+      <c r="D149" s="137"/>
+      <c r="E149" s="137"/>
+      <c r="F149" s="137"/>
+      <c r="G149" s="137"/>
       <c r="H149" s="5"/>
       <c r="I149" s="5"/>
       <c r="J149" s="5"/>
@@ -28109,7 +28103,7 @@
       </c>
       <c r="F185" s="106"/>
       <c r="G185" s="5"/>
-      <c r="H185" s="139" t="s">
+      <c r="H185" s="136" t="s">
         <v>852</v>
       </c>
       <c r="I185" s="5"/>
@@ -28147,7 +28141,7 @@
       </c>
       <c r="F186" s="106"/>
       <c r="G186" s="5"/>
-      <c r="H186" s="140"/>
+      <c r="H186" s="137"/>
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
       <c r="K186" s="5"/>

</xml_diff>